<commit_message>
[SCF 2025] Small Fixes Excel File
</commit_message>
<xml_diff>
--- a/tools/excel/scf/scf-2025.1.1.xlsx
+++ b/tools/excel/scf/scf-2025.1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\scf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109A9CE5-6F23-4F89-9777-93856C5096DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEBF41C-55B4-4379-B8C1-763CABC64CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="-13515" windowWidth="20850" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -16157,15 +16157,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -16246,22 +16247,6 @@
       </c>
       <c r="B10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -16271,15 +16256,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -16340,9 +16326,25 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -16355,9 +16357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A920" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D949" sqref="D949"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45741,6 +45743,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -45770,6 +45775,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>